<commit_message>
Added Sheet for Safe Mode
</commit_message>
<xml_diff>
--- a/CougSat1-PowerBoard/Documentation/Native/EnergyBudget.xlsx
+++ b/CougSat1-PowerBoard/Documentation/Native/EnergyBudget.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1-PowerBoard\Documentation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC5D811-97F6-4166-BB93-33171FF810D3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603A1B7-DDE3-4E9F-A090-C101486FBF72}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="27795" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orbit" sheetId="2" r:id="rId1"/>
+    <sheet name="Safe Mode Orbit" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Time in Eclipse</t>
   </si>
@@ -80,9 +81,6 @@
   </si>
   <si>
     <t>Model</t>
-  </si>
-  <si>
-    <t>Mode</t>
   </si>
   <si>
     <t>STM32L496 @ 80 MHz</t>
@@ -164,21 +162,24 @@
   <si>
     <t>Heaters</t>
   </si>
+  <si>
+    <t>Coug Sat-1 Orbital Energy Budget (Safe Mode)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="165" formatCode="0.0\ &quot;hrs/day&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.00\ &quot;Wh&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.00\ &quot;W&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.0\ &quot;hours&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.0\ &quot;hr&quot;"/>
-    <numFmt numFmtId="170" formatCode="0.000\ &quot;Wh&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.00\ &quot;hr&quot;"/>
-    <numFmt numFmtId="172" formatCode="0.0\ &quot;W&quot;"/>
-    <numFmt numFmtId="174" formatCode="0.00\ &quot;Panels&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.0\ &quot;hrs/day&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.00\ &quot;Wh&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00\ &quot;W&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.0\ &quot;hours&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.0\ &quot;hr&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.000\ &quot;Wh&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.00\ &quot;hr&quot;"/>
+    <numFmt numFmtId="171" formatCode="0.0\ &quot;W&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00\ &quot;Panels&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -314,27 +315,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="172" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -342,13 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="174" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -358,37 +360,7 @@
     <cellStyle name="Output" xfId="2" builtinId="21"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -460,72 +432,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1876425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>363085</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="http://www.apricus.com/upload/userfiles/images/flat-plate-IAM.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC371399-E5F3-4615-BB8E-5F77D7D010F7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6562725" y="0"/>
-          <a:ext cx="2343150" cy="1934710"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -853,7 +759,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,116 +776,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="13">
         <f>D6*D5*D7*D3</f>
         <v>2.9063399399999996</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="7">
         <f>18/16</f>
         <v>1.125</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="17"/>
+      <c r="E3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>35</v>
+      <c r="A4" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B4" s="13">
         <f>SUM(E10:E53)*D3/SUM(D3:D4)</f>
         <v>2.1391800000000001</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="6">
         <f>6/16</f>
         <v>0.375</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="17"/>
+      <c r="E4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>36</v>
+      <c r="A5" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="13">
         <f>SUM(E10:E53)*D4/SUM(D3:D4)</f>
         <v>0.71306000000000003</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <v>1.4</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="17"/>
+      <c r="E5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <f>B3-SUM(B4:B5)</f>
         <v>5.4099939999999513E-2</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="14">
         <f>2*2.35*16.4/1000*26.6</f>
         <v>2.0503279999999999</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="17"/>
+      <c r="E6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="21" t="s">
-        <v>30</v>
+      <c r="C7" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="4">
         <v>0.9</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="17"/>
+      <c r="E7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="22"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -992,7 +898,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>6</v>
@@ -1000,9 +906,7 @@
       <c r="F9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1019,11 +923,11 @@
         <v>1.5</v>
       </c>
       <c r="E10" s="11">
-        <f>IF(C10&lt;&gt;0,B10*D10,"")</f>
+        <f t="shared" ref="E10:E44" si="1">IF(C10&lt;&gt;0,B10*D10,"")</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8"/>
     </row>
@@ -1042,16 +946,16 @@
         <v>1.5</v>
       </c>
       <c r="E11" s="11">
-        <f>IF(C11&lt;&gt;0,B11*D11,"")</f>
+        <f t="shared" si="1"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3">
         <v>0.48</v>
@@ -1064,13 +968,13 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="11">
-        <f>IF(C12&lt;&gt;0,B12*D12,"")</f>
+        <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -1084,13 +988,13 @@
         <v>0.2</v>
       </c>
       <c r="E13" s="11">
-        <f>IF(C13&lt;&gt;0,B13*D13,"")</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -1104,7 +1008,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="E14" s="11">
-        <f>IF(C14&lt;&gt;0,B14*D14,"")</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
@@ -1123,11 +1027,11 @@
         <v>1.5</v>
       </c>
       <c r="E15" s="11">
-        <f>IF(C15&lt;&gt;0,B15*D15,"")</f>
+        <f t="shared" si="1"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1145,7 +1049,7 @@
         <v>0.75</v>
       </c>
       <c r="E16" s="11">
-        <f>IF(C16&lt;&gt;0,B16*D16,"")</f>
+        <f t="shared" si="1"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="F16" t="s">
@@ -1169,11 +1073,11 @@
         <v>1.5</v>
       </c>
       <c r="E17" s="11">
-        <f>IF(C17&lt;&gt;0,B17*D17,"")</f>
+        <f t="shared" si="1"/>
         <v>0.24354000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,7 +1097,7 @@
         <v>1.5</v>
       </c>
       <c r="E18" s="11">
-        <f>IF(C18&lt;&gt;0,B18*D18,"")</f>
+        <f t="shared" si="1"/>
         <v>0.16335</v>
       </c>
     </row>
@@ -1213,16 +1117,16 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="E19" s="11">
-        <f>IF(C19&lt;&gt;0,B19*D19,"")</f>
+        <f t="shared" si="1"/>
         <v>3.960000000000001E-2</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3">
         <v>2</v>
@@ -1236,7 +1140,7 @@
         <v>0.25</v>
       </c>
       <c r="E20" s="11">
-        <f>IF(C20&lt;&gt;0,B20*D20,"")</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="F20" t="s">
@@ -1245,7 +1149,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3">
         <f>0.27*3</f>
@@ -1259,16 +1163,16 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="E21" s="11">
-        <f>IF(C21&lt;&gt;0,B21*D21,"")</f>
+        <f t="shared" si="1"/>
         <v>6.0750000000000012E-2</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="3">
         <v>0.25</v>
@@ -1281,11 +1185,11 @@
         <v>1.5</v>
       </c>
       <c r="E22" s="11">
-        <f>IF(C22&lt;&gt;0,B22*D22,"")</f>
+        <f t="shared" si="1"/>
         <v>0.375</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,7 +1200,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E23" s="11" t="str">
-        <f>IF(C23&lt;&gt;0,B23*D23,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1308,7 +1212,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E24" s="11" t="str">
-        <f>IF(C24&lt;&gt;0,B24*D24,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1320,7 +1224,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E25" s="11" t="str">
-        <f>IF(C25&lt;&gt;0,B25*D25,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1332,7 +1236,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="11" t="str">
-        <f>IF(C26&lt;&gt;0,B26*D26,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1344,7 +1248,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E27" s="11" t="str">
-        <f>IF(C27&lt;&gt;0,B27*D27,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1356,7 +1260,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E28" s="11" t="str">
-        <f>IF(C28&lt;&gt;0,B28*D28,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1368,7 +1272,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E29" s="11" t="str">
-        <f>IF(C29&lt;&gt;0,B29*D29,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1380,7 +1284,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E30" s="11" t="str">
-        <f>IF(C30&lt;&gt;0,B30*D30,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1392,7 +1296,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E31" s="11" t="str">
-        <f>IF(C31&lt;&gt;0,B31*D31,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1404,7 +1308,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E32" s="11" t="str">
-        <f>IF(C32&lt;&gt;0,B32*D32,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1416,7 +1320,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E33" s="11" t="str">
-        <f>IF(C33&lt;&gt;0,B33*D33,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1428,7 +1332,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E34" s="11" t="str">
-        <f>IF(C34&lt;&gt;0,B34*D34,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1440,7 +1344,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E35" s="11" t="str">
-        <f>IF(C35&lt;&gt;0,B35*D35,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1452,7 +1356,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E36" s="11" t="str">
-        <f>IF(C36&lt;&gt;0,B36*D36,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1464,7 +1368,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E37" s="11" t="str">
-        <f>IF(C37&lt;&gt;0,B37*D37,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1476,7 +1380,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" s="11" t="str">
-        <f>IF(C38&lt;&gt;0,B38*D38,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1488,7 +1392,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E39" s="11" t="str">
-        <f>IF(C39&lt;&gt;0,B39*D39,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1500,7 +1404,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E40" s="11" t="str">
-        <f>IF(C40&lt;&gt;0,B40*D40,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1512,7 +1416,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="11" t="str">
-        <f>IF(C41&lt;&gt;0,B41*D41,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1524,7 +1428,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E42" s="11" t="str">
-        <f>IF(C42&lt;&gt;0,B42*D42,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1536,7 +1440,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="11" t="str">
-        <f>IF(C43&lt;&gt;0,B43*D43,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1548,7 +1452,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E44" s="11" t="str">
-        <f>IF(C44&lt;&gt;0,B44*D44,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1560,7 +1464,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E45" s="2" t="str">
-        <f>IF(B45*C45&lt;&gt;0,B45*C45,"")</f>
+        <f t="shared" ref="E45:E53" si="2">IF(B45*C45&lt;&gt;0,B45*C45,"")</f>
         <v/>
       </c>
     </row>
@@ -1572,7 +1476,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E46" s="2" t="str">
-        <f>IF(B46*C46&lt;&gt;0,B46*C46,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1581,7 +1485,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="1"/>
       <c r="E47" s="2" t="str">
-        <f>IF(B47*C47&lt;&gt;0,B47*C47,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1590,7 +1494,7 @@
       <c r="C48" s="9"/>
       <c r="D48" s="1"/>
       <c r="E48" s="2" t="str">
-        <f>IF(B48*C48&lt;&gt;0,B48*C48,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1599,7 +1503,7 @@
       <c r="C49" s="9"/>
       <c r="D49" s="1"/>
       <c r="E49" s="2" t="str">
-        <f>IF(B49*C49&lt;&gt;0,B49*C49,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1608,7 +1512,7 @@
       <c r="C50" s="9"/>
       <c r="D50" s="1"/>
       <c r="E50" s="2" t="str">
-        <f>IF(B50*C50&lt;&gt;0,B50*C50,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1617,7 +1521,7 @@
       <c r="C51" s="9"/>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="str">
-        <f>IF(B51*C51&lt;&gt;0,B51*C51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1626,7 +1530,7 @@
       <c r="C52" s="9"/>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="str">
-        <f>IF(B52*C52&lt;&gt;0,B52*C52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1635,7 +1539,7 @@
       <c r="C53" s="9"/>
       <c r="D53" s="1"/>
       <c r="E53" s="2" t="str">
-        <f>IF(B53*C53&lt;&gt;0,B53*C53,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1680,14 +1584,14 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="between">
       <formula>0</formula>
       <formula>$B$3*0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThan">
       <formula>$B$3*0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1717,6 +1621,874 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7829720D-C79F-49CF-AAEE-45D1A431B3C7}">
+  <dimension ref="A1:G63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="16"/>
+    <col min="9" max="9" width="14.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13">
+        <f>D6*D5*D7*D3</f>
+        <v>2.9063399399999996</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <f>18/16</f>
+        <v>1.125</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="13">
+        <f>SUM(E10:E53)*D3/SUM(D3:D4)</f>
+        <v>1.243125</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <f>6/16</f>
+        <v>0.375</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="13">
+        <f>SUM(E10:E53)*D4/SUM(D3:D4)</f>
+        <v>0.41437499999999999</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1.4</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <f>B3-SUM(B4:B5)</f>
+        <v>1.2488399399999996</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14">
+        <f>2*2.35*16.4/1000*26.6</f>
+        <v>2.0503279999999999</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" ref="D10:D13" si="0">IF(OR(C10*($D$3+$D$4)&lt;&gt;0,B10&lt;&gt;0),C10*($D$3+$D$4)," ")</f>
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" ref="E10:E13" si="1">IF(C10&lt;&gt;"",B10*D10,"")</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <f>4/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <f>IF(OR(C14*($D$3+$D$4)&lt;&gt;0,B14&lt;&gt;0),C14*($D$3+$D$4)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
+        <f>IF(C14&lt;&gt;"",B14*D14,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" ref="D15:D46" si="2">IF(OR(C15*($D$3+$D$4)&lt;&gt;0,B15&lt;&gt;0),C15*($D$3+$D$4)," ")</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" ref="E15:E46" si="3">IF(C15&lt;&gt;"",B15*D15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
+        <f>3.3*0.0123*4</f>
+        <v>0.16236</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="3">
+        <f>0.033*3.3</f>
+        <v>0.1089</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3">
+        <f>3.3*0.08</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9">
+        <f>D4/D3/2</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D20" s="12">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3">
+        <f>0.27*3</f>
+        <v>0.81</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="3"/>
+        <v>0.1875</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E23" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E24" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E25" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E26" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E27" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E28" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E29" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E30" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E31" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E32" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E33" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E34" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E35" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E36" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E37" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E38" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E39" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E40" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E41" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E42" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E43" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E44" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E45" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E46" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2" t="str">
+        <f t="shared" ref="E45:E53" si="4">IF(B47*C47&lt;&gt;0,B47*C47,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C59" s="9"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C61" s="9"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C63" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>$B$3*0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>$B$3*0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D55">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added JTAG Disconnector and LEDs
</commit_message>
<xml_diff>
--- a/CougSat1-PowerBoard/Documentation/Native/EnergyBudget.xlsx
+++ b/CougSat1-PowerBoard/Documentation/Native/EnergyBudget.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1-PowerBoard\Documentation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA3BA6F-B99B-42FB-894C-09C643B6761C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BE35D6-02C5-471D-836E-716111EA0BED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="27795" windowHeight="12855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,10 @@
     <sheet name="Orbit" sheetId="2" r:id="rId1"/>
     <sheet name="Safe Mode Orbit" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Orbit!$A$1:$I$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Safe Mode Orbit'!$A$1:$I$30</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
@@ -373,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -438,6 +442,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -446,23 +493,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -474,18 +514,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -493,11 +530,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -506,37 +569,7 @@
     <cellStyle name="Output" xfId="2" builtinId="21"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -935,20 +968,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -978,1095 +1011,1103 @@
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <f>E6*E5*E3</f>
         <v>3.2292665999999994</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="6">
+      <c r="D3" s="23"/>
+      <c r="E3" s="5">
         <f>18/16</f>
         <v>1.125</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <f>SUM(H11:H54)*E3/SUM(E3:E4)</f>
         <v>1.8027867187500002</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="5">
+      <c r="C4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="4">
         <f>6/16</f>
         <v>0.375</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <f>SUM(H11:H54)*E4/SUM(E3:E4)</f>
         <v>0.60092890625000006</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="15">
+      <c r="D5" s="23"/>
+      <c r="E5" s="12">
         <v>1.4</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <f>B3-SUM(B4:B5)</f>
         <v>0.82555097499999919</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="13">
+      <c r="D6" s="23"/>
+      <c r="E6" s="10">
         <f>2*2.35*16.4/1000*26.6</f>
         <v>2.0503279999999999</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="18"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="44" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="37">
         <v>3.3</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="38">
         <v>30</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="39">
         <f>C10*D10</f>
         <v>99</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="40">
         <v>1</v>
       </c>
-      <c r="G10" s="11">
-        <f>F10*($E$3+$E$4)</f>
+      <c r="G10" s="41">
+        <f t="shared" ref="G10:G30" si="0">F10*($E$3+$E$4)</f>
         <v>1.5</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="42">
         <f>E10*G10/1000</f>
         <v>0.14849999999999999</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="43"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="26">
         <v>3.3</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="27">
         <v>20</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="28">
         <f>C11*D11</f>
         <v>66</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="29">
         <v>1</v>
       </c>
-      <c r="G11" s="11">
-        <f>F11*($E$3+$E$4)</f>
+      <c r="G11" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="31">
         <f>E11*G11/1000</f>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="26">
         <v>3.3</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="27">
         <v>60</v>
       </c>
-      <c r="E12" s="24">
-        <f t="shared" ref="E12:E30" si="0">C12*D12</f>
+      <c r="E12" s="28">
+        <f t="shared" ref="E12:E30" si="1">C12*D12</f>
         <v>198</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="29">
         <v>0.1</v>
       </c>
-      <c r="G12" s="11">
-        <f>F12*($E$3+$E$4)</f>
+      <c r="G12" s="30">
+        <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="H12" s="10">
-        <f t="shared" ref="H12:H30" si="1">E12*G12/1000</f>
+      <c r="H12" s="31">
+        <f t="shared" ref="H12:H30" si="2">E12*G12/1000</f>
         <v>2.9700000000000004E-2</v>
       </c>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="26">
         <v>3.3</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="27">
         <v>20</v>
       </c>
-      <c r="E13" s="24">
-        <f t="shared" si="0"/>
+      <c r="E13" s="28">
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="29">
         <v>1</v>
       </c>
-      <c r="G13" s="11">
-        <f>F13*($E$3+$E$4)</f>
+      <c r="G13" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H13" s="10">
-        <f t="shared" si="1"/>
+      <c r="H13" s="31">
+        <f t="shared" si="2"/>
         <v>9.9000000000000005E-2</v>
       </c>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="26">
         <v>3.3</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="27">
         <v>45</v>
       </c>
-      <c r="E14" s="24">
-        <f t="shared" si="0"/>
+      <c r="E14" s="28">
+        <f t="shared" si="1"/>
         <v>148.5</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="29">
         <v>1</v>
       </c>
-      <c r="G14" s="11">
-        <f>F14*($E$3+$E$4)</f>
+      <c r="G14" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H14" s="10">
-        <f t="shared" si="1"/>
+      <c r="H14" s="31">
+        <f t="shared" si="2"/>
         <v>0.22275</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="26">
         <v>3.3</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="27">
         <v>55</v>
       </c>
-      <c r="E15" s="24">
-        <f t="shared" si="0"/>
+      <c r="E15" s="28">
+        <f t="shared" si="1"/>
         <v>181.5</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="29">
         <v>1</v>
       </c>
-      <c r="G15" s="11">
-        <f>F15*($E$3+$E$4)</f>
+      <c r="G15" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H15" s="10">
-        <f t="shared" si="1"/>
+      <c r="H15" s="31">
+        <f t="shared" si="2"/>
         <v>0.27224999999999999</v>
       </c>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="26">
         <v>3.3</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="27">
         <v>90</v>
       </c>
-      <c r="E16" s="24">
-        <f t="shared" si="0"/>
+      <c r="E16" s="28">
+        <f t="shared" si="1"/>
         <v>297</v>
       </c>
-      <c r="F16" s="31">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
-        <f>F16*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="F16" s="29">
+        <v>0</v>
+      </c>
+      <c r="G16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="32" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="26">
         <v>3.3</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="27">
         <v>105</v>
       </c>
-      <c r="E17" s="24">
-        <f t="shared" si="0"/>
+      <c r="E17" s="28">
+        <f t="shared" si="1"/>
         <v>346.5</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="29">
         <v>1</v>
       </c>
-      <c r="G17" s="11">
-        <f>F17*($E$3+$E$4)</f>
+      <c r="G17" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H17" s="10">
-        <f t="shared" si="1"/>
+      <c r="H17" s="31">
+        <f t="shared" si="2"/>
         <v>0.51975000000000005</v>
       </c>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="26">
         <v>3.3</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="27">
         <v>50</v>
       </c>
-      <c r="E18" s="24">
-        <f t="shared" si="0"/>
+      <c r="E18" s="28">
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="29">
         <v>0.5</v>
       </c>
-      <c r="G18" s="11">
-        <f>F18*($E$3+$E$4)</f>
+      <c r="G18" s="30">
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H18" s="10">
-        <f t="shared" si="1"/>
+      <c r="H18" s="31">
+        <f t="shared" si="2"/>
         <v>0.12375</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="32" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="26">
         <v>3.3</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="27">
         <v>390</v>
       </c>
-      <c r="E19" s="24">
-        <f t="shared" si="0"/>
+      <c r="E19" s="28">
+        <f t="shared" si="1"/>
         <v>1287</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="33">
         <f>20/86400</f>
         <v>2.3148148148148149E-4</v>
       </c>
-      <c r="G19" s="11">
-        <f>F19*($E$3+$E$4)</f>
+      <c r="G19" s="30">
+        <f t="shared" si="0"/>
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="H19" s="10">
-        <f t="shared" si="1"/>
+      <c r="H19" s="31">
+        <f t="shared" si="2"/>
         <v>4.4687500000000001E-4</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="32" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="26">
         <v>3.3</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="27">
         <v>25</v>
       </c>
-      <c r="E20" s="24">
-        <f t="shared" si="0"/>
+      <c r="E20" s="28">
+        <f t="shared" si="1"/>
         <v>82.5</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="34">
         <f>10/3600</f>
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="G20" s="11">
-        <f>F20*($E$3+$E$4)</f>
+      <c r="G20" s="30">
+        <f t="shared" si="0"/>
         <v>4.1666666666666666E-3</v>
       </c>
-      <c r="H20" s="10">
-        <f t="shared" si="1"/>
+      <c r="H20" s="31">
+        <f t="shared" si="2"/>
         <v>3.4374999999999998E-4</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="26">
         <v>3.3</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="27">
         <v>15</v>
       </c>
-      <c r="E21" s="24">
-        <f t="shared" si="0"/>
+      <c r="E21" s="28">
+        <f t="shared" si="1"/>
         <v>49.5</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="35">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G21" s="11">
-        <f>F21*($E$3+$E$4)</f>
+      <c r="G21" s="30">
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="H21" s="10">
-        <f t="shared" si="1"/>
+      <c r="H21" s="31">
+        <f t="shared" si="2"/>
         <v>6.1875000000000003E-3</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="32" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="26">
         <v>3.3</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="27">
         <v>390</v>
       </c>
-      <c r="E22" s="24">
-        <f t="shared" si="0"/>
+      <c r="E22" s="28">
+        <f t="shared" si="1"/>
         <v>1287</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="29">
         <f>20/3600</f>
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="G22" s="11">
-        <f>F22*($E$3+$E$4)</f>
+      <c r="G22" s="30">
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="H22" s="10">
-        <f t="shared" si="1"/>
+      <c r="H22" s="31">
+        <f t="shared" si="2"/>
         <v>1.0725E-2</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="32" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="22">
+      <c r="B23" s="32"/>
+      <c r="C23" s="26">
         <v>3.3</v>
       </c>
-      <c r="D23" s="23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="31">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
-        <f>F23*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D23" s="27">
+        <v>0</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="26">
         <v>3.7</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="27">
         <v>100</v>
       </c>
-      <c r="E24" s="24">
-        <f t="shared" si="0"/>
+      <c r="E24" s="28">
+        <f t="shared" si="1"/>
         <v>370</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="29">
         <v>0.5</v>
       </c>
-      <c r="G24" s="11">
-        <f>F24*($E$3+$E$4)</f>
+      <c r="G24" s="30">
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H24" s="10">
-        <f t="shared" si="1"/>
+      <c r="H24" s="31">
+        <f t="shared" si="2"/>
         <v>0.27750000000000002</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="26">
         <v>3.7</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="27">
         <v>250</v>
       </c>
-      <c r="E25" s="24">
-        <f t="shared" si="0"/>
+      <c r="E25" s="28">
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="29">
         <f>E4/(E3+E4)/2</f>
         <v>0.125</v>
       </c>
-      <c r="G25" s="11">
-        <f>F25*($E$3+$E$4)</f>
+      <c r="G25" s="30">
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="H25" s="10">
-        <f t="shared" si="1"/>
+      <c r="H25" s="31">
+        <f t="shared" si="2"/>
         <v>0.17343749999999999</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="26">
         <v>3.7</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="27">
         <v>250</v>
       </c>
-      <c r="E26" s="24">
-        <f t="shared" si="0"/>
+      <c r="E26" s="28">
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="29">
         <f>E4/(E3+E4)/2</f>
         <v>0.125</v>
       </c>
-      <c r="G26" s="11">
-        <f>F26*($E$3+$E$4)</f>
+      <c r="G26" s="30">
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="H26" s="10">
-        <f t="shared" si="1"/>
+      <c r="H26" s="31">
+        <f t="shared" si="2"/>
         <v>0.17343749999999999</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="26">
         <v>3.7</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="27">
         <v>300</v>
       </c>
-      <c r="E27" s="24">
-        <f t="shared" si="0"/>
+      <c r="E27" s="28">
+        <f t="shared" si="1"/>
         <v>1110</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="29">
         <f>8/60</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="G27" s="11">
-        <f>F27*($E$3+$E$4)</f>
+      <c r="G27" s="30">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="H27" s="10">
-        <f t="shared" si="1"/>
+      <c r="H27" s="31">
+        <f t="shared" si="2"/>
         <v>0.222</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="32" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="26">
         <v>3.7</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="27">
         <v>1000</v>
       </c>
-      <c r="E28" s="24">
-        <f t="shared" si="0"/>
+      <c r="E28" s="28">
+        <f t="shared" si="1"/>
         <v>3700</v>
       </c>
-      <c r="F28" s="31">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <f>F28*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="F28" s="29">
+        <v>0</v>
+      </c>
+      <c r="G28" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="32" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="26">
         <v>3.7</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="27">
         <v>250</v>
       </c>
-      <c r="E29" s="24">
-        <f t="shared" si="0"/>
+      <c r="E29" s="28">
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="29">
         <f>E4/(E3+E4)/2</f>
         <v>0.125</v>
       </c>
-      <c r="G29" s="11">
-        <f>F29*($E$3+$E$4)</f>
+      <c r="G29" s="30">
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="H29" s="10">
-        <f t="shared" si="1"/>
+      <c r="H29" s="31">
+        <f t="shared" si="2"/>
         <v>0.17343749999999999</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I29" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="22">
+      <c r="B30" s="32"/>
+      <c r="C30" s="26">
         <v>3.7</v>
       </c>
-      <c r="D30" s="23">
-        <v>0</v>
-      </c>
-      <c r="E30" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="31">
-        <v>0</v>
-      </c>
-      <c r="G30" s="11">
-        <f>F30*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D30" s="27">
+        <v>0</v>
+      </c>
+      <c r="E30" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="29">
+        <v>0</v>
+      </c>
+      <c r="G30" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9" t="str">
-        <f>IF(F31*($E$3+$E$4)&lt;&gt;0, F31*($E$3+$E$4), " ")</f>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7" t="str">
+        <f t="shared" ref="G31:G37" si="3">IF(F31*($E$3+$E$4)&lt;&gt;0, F31*($E$3+$E$4), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H31" s="10" t="str">
-        <f t="shared" ref="H31:H45" si="2">IF(F31&lt;&gt;0,E31*G31,"")</f>
+      <c r="H31" s="8" t="str">
+        <f t="shared" ref="H31:H45" si="4">IF(F31&lt;&gt;0,E31*G31,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9" t="str">
-        <f>IF(F32*($E$3+$E$4)&lt;&gt;0, F32*($E$3+$E$4), " ")</f>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H32" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H32" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9" t="str">
-        <f>IF(F33*($E$3+$E$4)&lt;&gt;0, F33*($E$3+$E$4), " ")</f>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H33" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H33" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9" t="str">
-        <f>IF(F34*($E$3+$E$4)&lt;&gt;0, F34*($E$3+$E$4), " ")</f>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H34" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H34" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9" t="str">
-        <f>IF(F35*($E$3+$E$4)&lt;&gt;0, F35*($E$3+$E$4), " ")</f>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H35" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H35" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="9" t="str">
-        <f>IF(F36*($E$3+$E$4)&lt;&gt;0, F36*($E$3+$E$4), " ")</f>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H36" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H36" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37" s="3"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="9" t="str">
-        <f>IF(F37*($E$3+$E$4)&lt;&gt;0, F37*($E$3+$E$4), " ")</f>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H37" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H37" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="9" t="str">
-        <f>IF(F39*($E$3+$E$4)&lt;&gt;0, F39*($E$3+$E$4), " ")</f>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7" t="str">
+        <f t="shared" ref="G39:G47" si="5">IF(F39*($E$3+$E$4)&lt;&gt;0, F39*($E$3+$E$4), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H39" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H39" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E40" s="3"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="9" t="str">
-        <f>IF(F40*($E$3+$E$4)&lt;&gt;0, F40*($E$3+$E$4), " ")</f>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H40" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H40" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E41" s="3"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="9" t="str">
-        <f>IF(F41*($E$3+$E$4)&lt;&gt;0, F41*($E$3+$E$4), " ")</f>
+      <c r="F41" s="6"/>
+      <c r="G41" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H41" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H41" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9" t="str">
-        <f>IF(F42*($E$3+$E$4)&lt;&gt;0, F42*($E$3+$E$4), " ")</f>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H42" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H42" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9" t="str">
-        <f>IF(F43*($E$3+$E$4)&lt;&gt;0, F43*($E$3+$E$4), " ")</f>
+      <c r="F43" s="6"/>
+      <c r="G43" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H43" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H43" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9" t="str">
-        <f>IF(F44*($E$3+$E$4)&lt;&gt;0, F44*($E$3+$E$4), " ")</f>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H44" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H44" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E45" s="3"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9" t="str">
-        <f>IF(F45*($E$3+$E$4)&lt;&gt;0, F45*($E$3+$E$4), " ")</f>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H45" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H45" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E46" s="3"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9" t="str">
-        <f>IF(F46*($E$3+$E$4)&lt;&gt;0, F46*($E$3+$E$4), " ")</f>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H46" s="2" t="str">
-        <f t="shared" ref="H46:H54" si="3">IF(E46*F46&lt;&gt;0,E46*F46,"")</f>
+        <f t="shared" ref="H46:H54" si="6">IF(E46*F46&lt;&gt;0,E46*F46,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E47" s="3"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9" t="str">
-        <f>IF(F47*($E$3+$E$4)&lt;&gt;0, F47*($E$3+$E$4), " ")</f>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H47" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E48" s="3"/>
-      <c r="F48" s="8"/>
+      <c r="F48" s="6"/>
       <c r="G48" s="1"/>
       <c r="H48" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E49" s="3"/>
-      <c r="F49" s="8"/>
+      <c r="F49" s="6"/>
       <c r="G49" s="1"/>
       <c r="H49" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E50" s="3"/>
-      <c r="F50" s="8"/>
+      <c r="F50" s="6"/>
       <c r="G50" s="1"/>
       <c r="H50" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E51" s="3"/>
-      <c r="F51" s="8"/>
+      <c r="F51" s="6"/>
       <c r="G51" s="1"/>
       <c r="H51" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E52" s="3"/>
-      <c r="F52" s="8"/>
+      <c r="F52" s="6"/>
       <c r="G52" s="1"/>
       <c r="H52" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E53" s="3"/>
-      <c r="F53" s="8"/>
+      <c r="F53" s="6"/>
       <c r="G53" s="1"/>
       <c r="H53" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E54" s="3"/>
-      <c r="F54" s="8"/>
+      <c r="F54" s="6"/>
       <c r="G54" s="1"/>
       <c r="H54" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F55" s="8"/>
+      <c r="F55" s="6"/>
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F56" s="8"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F57" s="8"/>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F58" s="8"/>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F59" s="8"/>
+      <c r="F59" s="6"/>
     </row>
     <row r="60" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F60" s="8"/>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F61" s="8"/>
+      <c r="F61" s="6"/>
     </row>
     <row r="62" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F62" s="8"/>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F63" s="8"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F64" s="8"/>
+      <c r="F64" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <conditionalFormatting sqref="B6">
     <cfRule type="cellIs" dxfId="5" priority="11" operator="between">
@@ -2116,8 +2157,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2127,24 +2168,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="18"/>
-    <col min="11" max="11" width="14.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="15"/>
+    <col min="11" max="11" width="14.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2172,1054 +2213,1069 @@
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <f>E6*E5*E3</f>
         <v>3.2292665999999994</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="6">
+      <c r="D3" s="23"/>
+      <c r="E3" s="5">
         <f>18/16</f>
         <v>1.125</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <f>SUM(H11:H54)*E3/SUM(E3:E4)</f>
         <v>0.91127812499999994</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="5">
+      <c r="C4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="4">
         <f>6/16</f>
         <v>0.375</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <f>SUM(H11:H54)*E4/SUM(E3:E4)</f>
         <v>0.303759375</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="15">
+      <c r="D5" s="23"/>
+      <c r="E5" s="12">
         <v>1.4</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <f>B3-SUM(B4:B5)</f>
         <v>2.0142290999999997</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="13">
+      <c r="D6" s="23"/>
+      <c r="E6" s="10">
         <f>2*2.35*16.4/1000*26.6</f>
         <v>2.0503279999999999</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="44" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="37">
         <v>3.3</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="38">
         <v>30</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="39">
         <f>C10*D10</f>
         <v>99</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="40">
         <v>1</v>
       </c>
-      <c r="G10" s="11">
-        <f>F10*($E$3+$E$4)</f>
+      <c r="G10" s="41">
+        <f t="shared" ref="G10:G30" si="0">F10*($E$3+$E$4)</f>
         <v>1.5</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="42">
         <f>E10*G10/1000</f>
         <v>0.14849999999999999</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="43"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="26">
         <v>3.3</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="27">
         <v>20</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="28">
         <f>C11*D11</f>
         <v>66</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="29">
         <v>1</v>
       </c>
-      <c r="G11" s="11">
-        <f>F11*($E$3+$E$4)</f>
+      <c r="G11" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="31">
         <f>E11*G11/1000</f>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="26">
         <v>3.3</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="27">
         <v>60</v>
       </c>
-      <c r="E12" s="24">
-        <f t="shared" ref="E12:E30" si="0">C12*D12</f>
+      <c r="E12" s="28">
+        <f t="shared" ref="E12:E30" si="1">C12*D12</f>
         <v>198</v>
       </c>
-      <c r="F12" s="31">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11">
-        <f>F12*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" ref="H12:H30" si="1">E12*G12/1000</f>
-        <v>0</v>
-      </c>
+      <c r="F12" s="29">
+        <v>0</v>
+      </c>
+      <c r="G12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
+        <f t="shared" ref="H12:H30" si="2">E12*G12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="26">
         <v>3.3</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="27">
         <v>20</v>
       </c>
-      <c r="E13" s="24">
-        <f t="shared" si="0"/>
+      <c r="E13" s="28">
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="29">
         <v>0.5</v>
       </c>
-      <c r="G13" s="11">
-        <f>F13*($E$3+$E$4)</f>
+      <c r="G13" s="30">
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H13" s="10">
-        <f t="shared" si="1"/>
+      <c r="H13" s="31">
+        <f t="shared" si="2"/>
         <v>4.9500000000000002E-2</v>
       </c>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="26">
         <v>3.3</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="27">
         <v>45</v>
       </c>
-      <c r="E14" s="24">
-        <f t="shared" si="0"/>
+      <c r="E14" s="28">
+        <f t="shared" si="1"/>
         <v>148.5</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="29">
         <v>0.15</v>
       </c>
-      <c r="G14" s="11">
-        <f>F14*($E$3+$E$4)</f>
+      <c r="G14" s="30">
+        <f t="shared" si="0"/>
         <v>0.22499999999999998</v>
       </c>
-      <c r="H14" s="10">
-        <f t="shared" si="1"/>
+      <c r="H14" s="31">
+        <f t="shared" si="2"/>
         <v>3.3412499999999998E-2</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="26">
         <v>3.3</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="27">
         <v>55</v>
       </c>
-      <c r="E15" s="24">
-        <f t="shared" si="0"/>
+      <c r="E15" s="28">
+        <f t="shared" si="1"/>
         <v>181.5</v>
       </c>
-      <c r="F15" s="31">
-        <v>0</v>
-      </c>
-      <c r="G15" s="11">
-        <f>F15*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F15" s="29">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="26">
         <v>3.3</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="27">
         <v>90</v>
       </c>
-      <c r="E16" s="24">
-        <f t="shared" si="0"/>
+      <c r="E16" s="28">
+        <f t="shared" si="1"/>
         <v>297</v>
       </c>
-      <c r="F16" s="31">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
-        <f>F16*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F16" s="29">
+        <v>0</v>
+      </c>
+      <c r="G16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="26">
         <v>3.3</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="27">
         <v>105</v>
       </c>
-      <c r="E17" s="24">
-        <f t="shared" si="0"/>
+      <c r="E17" s="28">
+        <f t="shared" si="1"/>
         <v>346.5</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="29">
         <v>1</v>
       </c>
-      <c r="G17" s="11">
-        <f>F17*($E$3+$E$4)</f>
+      <c r="G17" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H17" s="10">
-        <f t="shared" si="1"/>
+      <c r="H17" s="31">
+        <f t="shared" si="2"/>
         <v>0.51975000000000005</v>
       </c>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="26">
         <v>3.3</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="27">
         <v>50</v>
       </c>
-      <c r="E18" s="24">
-        <f t="shared" si="0"/>
+      <c r="E18" s="28">
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
-      <c r="F18" s="31">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <f>F18*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F18" s="29">
+        <v>0</v>
+      </c>
+      <c r="G18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="26">
         <v>3.3</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="27">
         <v>390</v>
       </c>
-      <c r="E19" s="24">
-        <f t="shared" si="0"/>
+      <c r="E19" s="28">
+        <f t="shared" si="1"/>
         <v>1287</v>
       </c>
-      <c r="F19" s="30">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <f>F19*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="26">
         <v>3.3</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="27">
         <v>25</v>
       </c>
-      <c r="E20" s="24">
-        <f t="shared" si="0"/>
+      <c r="E20" s="28">
+        <f t="shared" si="1"/>
         <v>82.5</v>
       </c>
-      <c r="F20" s="29">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
-        <f>F20*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F20" s="34">
+        <v>0</v>
+      </c>
+      <c r="G20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="26">
         <v>3.3</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="27">
         <v>15</v>
       </c>
-      <c r="E21" s="24">
-        <f t="shared" si="0"/>
+      <c r="E21" s="28">
+        <f t="shared" si="1"/>
         <v>49.5</v>
       </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <f>F21*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F21" s="35">
+        <v>0</v>
+      </c>
+      <c r="G21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="26">
         <v>3.3</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="27">
         <v>390</v>
       </c>
-      <c r="E22" s="24">
-        <f t="shared" si="0"/>
+      <c r="E22" s="28">
+        <f t="shared" si="1"/>
         <v>1287</v>
       </c>
-      <c r="F22" s="31">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <f>F22*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F22" s="29">
+        <v>0</v>
+      </c>
+      <c r="G22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="22">
+      <c r="B23" s="32"/>
+      <c r="C23" s="26">
         <v>3.3</v>
       </c>
-      <c r="D23" s="23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="31">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
-        <f>F23*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D23" s="27">
+        <v>0</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="26">
         <v>3.7</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="27">
         <v>100</v>
       </c>
-      <c r="E24" s="24">
-        <f t="shared" si="0"/>
+      <c r="E24" s="28">
+        <f t="shared" si="1"/>
         <v>370</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="29">
         <v>0.1</v>
       </c>
-      <c r="G24" s="11">
-        <f>F24*($E$3+$E$4)</f>
+      <c r="G24" s="30">
+        <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="H24" s="10">
-        <f t="shared" si="1"/>
+      <c r="H24" s="31">
+        <f t="shared" si="2"/>
         <v>5.5500000000000008E-2</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="26">
         <v>3.7</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="27">
         <v>250</v>
       </c>
-      <c r="E25" s="24">
-        <f t="shared" si="0"/>
+      <c r="E25" s="28">
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="29">
         <f>E4/(E3+E4)/2</f>
         <v>0.125</v>
       </c>
-      <c r="G25" s="11">
-        <f>F25*($E$3+$E$4)</f>
+      <c r="G25" s="30">
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="H25" s="10">
-        <f t="shared" si="1"/>
+      <c r="H25" s="31">
+        <f t="shared" si="2"/>
         <v>0.17343749999999999</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="26">
         <v>3.7</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="27">
         <v>250</v>
       </c>
-      <c r="E26" s="24">
-        <f t="shared" si="0"/>
+      <c r="E26" s="28">
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="29">
         <f>E4/(E3+E4)/2</f>
         <v>0.125</v>
       </c>
-      <c r="G26" s="11">
-        <f>F26*($E$3+$E$4)</f>
+      <c r="G26" s="30">
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="H26" s="10">
-        <f t="shared" si="1"/>
+      <c r="H26" s="31">
+        <f t="shared" si="2"/>
         <v>0.17343749999999999</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="26">
         <v>3.7</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="27">
         <v>300</v>
       </c>
-      <c r="E27" s="24">
-        <f t="shared" si="0"/>
+      <c r="E27" s="28">
+        <f t="shared" si="1"/>
         <v>1110</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="35">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="G27" s="11">
-        <f>F27*($E$3+$E$4)</f>
+      <c r="G27" s="30">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H27" s="10">
-        <f t="shared" si="1"/>
+      <c r="H27" s="31">
+        <f t="shared" si="2"/>
         <v>0.111</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="26">
         <v>3.7</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="27">
         <v>1000</v>
       </c>
-      <c r="E28" s="24">
-        <f t="shared" si="0"/>
+      <c r="E28" s="28">
+        <f t="shared" si="1"/>
         <v>3700</v>
       </c>
-      <c r="F28" s="31">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <f>F28*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F28" s="29">
+        <v>0</v>
+      </c>
+      <c r="G28" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="26">
         <v>3.7</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="27">
         <v>250</v>
       </c>
-      <c r="E29" s="24">
-        <f t="shared" si="0"/>
+      <c r="E29" s="28">
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
-      <c r="F29" s="31">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
-        <f>F29*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="18" t="s">
+      <c r="F29" s="29">
+        <v>0</v>
+      </c>
+      <c r="G29" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="32" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="22">
+      <c r="B30" s="32"/>
+      <c r="C30" s="26">
         <v>3.7</v>
       </c>
-      <c r="D30" s="23">
-        <v>0</v>
-      </c>
-      <c r="E30" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="31">
-        <v>0</v>
-      </c>
-      <c r="G30" s="11">
-        <f>F30*($E$3+$E$4)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D30" s="27">
+        <v>0</v>
+      </c>
+      <c r="E30" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="29">
+        <v>0</v>
+      </c>
+      <c r="G30" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9" t="str">
-        <f>IF(F31*($E$3+$E$4)&lt;&gt;0, F31*($E$3+$E$4), " ")</f>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7" t="str">
+        <f t="shared" ref="G31:G37" si="3">IF(F31*($E$3+$E$4)&lt;&gt;0, F31*($E$3+$E$4), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H31" s="10" t="str">
-        <f t="shared" ref="H31:H45" si="2">IF(F31&lt;&gt;0,E31*G31,"")</f>
+      <c r="H31" s="8" t="str">
+        <f t="shared" ref="H31:H45" si="4">IF(F31&lt;&gt;0,E31*G31,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9" t="str">
-        <f>IF(F32*($E$3+$E$4)&lt;&gt;0, F32*($E$3+$E$4), " ")</f>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H32" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H32" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9" t="str">
-        <f>IF(F33*($E$3+$E$4)&lt;&gt;0, F33*($E$3+$E$4), " ")</f>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H33" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H33" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9" t="str">
-        <f>IF(F34*($E$3+$E$4)&lt;&gt;0, F34*($E$3+$E$4), " ")</f>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H34" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H34" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9" t="str">
-        <f>IF(F35*($E$3+$E$4)&lt;&gt;0, F35*($E$3+$E$4), " ")</f>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H35" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H35" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="9" t="str">
-        <f>IF(F36*($E$3+$E$4)&lt;&gt;0, F36*($E$3+$E$4), " ")</f>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H36" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H36" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37" s="3"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="9" t="str">
-        <f>IF(F37*($E$3+$E$4)&lt;&gt;0, F37*($E$3+$E$4), " ")</f>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H37" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H37" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="9" t="str">
-        <f>IF(F39*($E$3+$E$4)&lt;&gt;0, F39*($E$3+$E$4), " ")</f>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7" t="str">
+        <f t="shared" ref="G39:G47" si="5">IF(F39*($E$3+$E$4)&lt;&gt;0, F39*($E$3+$E$4), " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H39" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H39" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E40" s="3"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="9" t="str">
-        <f>IF(F40*($E$3+$E$4)&lt;&gt;0, F40*($E$3+$E$4), " ")</f>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H40" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H40" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E41" s="3"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="9" t="str">
-        <f>IF(F41*($E$3+$E$4)&lt;&gt;0, F41*($E$3+$E$4), " ")</f>
+      <c r="F41" s="6"/>
+      <c r="G41" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H41" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H41" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9" t="str">
-        <f>IF(F42*($E$3+$E$4)&lt;&gt;0, F42*($E$3+$E$4), " ")</f>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H42" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H42" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9" t="str">
-        <f>IF(F43*($E$3+$E$4)&lt;&gt;0, F43*($E$3+$E$4), " ")</f>
+      <c r="F43" s="6"/>
+      <c r="G43" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H43" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H43" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9" t="str">
-        <f>IF(F44*($E$3+$E$4)&lt;&gt;0, F44*($E$3+$E$4), " ")</f>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H44" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H44" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E45" s="3"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9" t="str">
-        <f>IF(F45*($E$3+$E$4)&lt;&gt;0, F45*($E$3+$E$4), " ")</f>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H45" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="H45" s="8" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E46" s="3"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9" t="str">
-        <f>IF(F46*($E$3+$E$4)&lt;&gt;0, F46*($E$3+$E$4), " ")</f>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H46" s="2" t="str">
-        <f t="shared" ref="H46:H54" si="3">IF(E46*F46&lt;&gt;0,E46*F46,"")</f>
+        <f t="shared" ref="H46:H54" si="6">IF(E46*F46&lt;&gt;0,E46*F46,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E47" s="3"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9" t="str">
-        <f>IF(F47*($E$3+$E$4)&lt;&gt;0, F47*($E$3+$E$4), " ")</f>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H47" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E48" s="3"/>
-      <c r="F48" s="8"/>
+      <c r="F48" s="6"/>
       <c r="G48" s="1"/>
       <c r="H48" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E49" s="3"/>
-      <c r="F49" s="8"/>
+      <c r="F49" s="6"/>
       <c r="G49" s="1"/>
       <c r="H49" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E50" s="3"/>
-      <c r="F50" s="8"/>
+      <c r="F50" s="6"/>
       <c r="G50" s="1"/>
       <c r="H50" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E51" s="3"/>
-      <c r="F51" s="8"/>
+      <c r="F51" s="6"/>
       <c r="G51" s="1"/>
       <c r="H51" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E52" s="3"/>
-      <c r="F52" s="8"/>
+      <c r="F52" s="6"/>
       <c r="G52" s="1"/>
       <c r="H52" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E53" s="3"/>
-      <c r="F53" s="8"/>
+      <c r="F53" s="6"/>
       <c r="G53" s="1"/>
       <c r="H53" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E54" s="3"/>
-      <c r="F54" s="8"/>
+      <c r="F54" s="6"/>
       <c r="G54" s="1"/>
       <c r="H54" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F55" s="8"/>
+      <c r="F55" s="6"/>
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F56" s="8"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F57" s="8"/>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F58" s="8"/>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F59" s="8"/>
+      <c r="F59" s="6"/>
     </row>
     <row r="60" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F60" s="8"/>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F61" s="8"/>
+      <c r="F61" s="6"/>
     </row>
     <row r="62" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F62" s="8"/>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F63" s="8"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F64" s="8"/>
+      <c r="F64" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3283,6 +3339,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>